<commit_message>
Se soluciono el problema al ingresar el usuario bien pero la contraseña incorrecta, y me muestra en la vista instructores solo los aprendices asignados segun su documento
</commit_message>
<xml_diff>
--- a/novedades.xlsx
+++ b/novedades.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,7 +438,7 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>45352</v>
+        <v>45355</v>
       </c>
     </row>
     <row r="3">
@@ -449,7 +449,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2711876</t>
+          <t>2556845</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>INTEGRACION DE CONTENIDOS DIGITALES.</t>
+          <t>DISEÑO E INTEGRACION DE MULTIMEDIA</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>45033</v>
+        <v>44760</v>
       </c>
     </row>
     <row r="7">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C7" s="1" t="n">
-        <v>45489</v>
+        <v>45124</v>
       </c>
     </row>
     <row r="8">
@@ -555,21 +555,21 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1096219906</v>
+        <v>1005178211</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CHARLES JAVIER</t>
+          <t>JUAN CAMILO</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>GALO CONTRERAS</t>
+          <t>DELGADO CARRASCAL</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>RETIRO VOLUNTARIO</t>
+          <t>CERTIFICADO</t>
         </is>
       </c>
     </row>
@@ -580,21 +580,21 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1096240059</v>
+        <v>1005181992</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MARIA PAULA</t>
+          <t>JOHAN</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ARTEAGA CARRILLO</t>
+          <t>VARGAS CALDERIN</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>RETIRO VOLUNTARIO</t>
+          <t>POR CERTIFICAR</t>
         </is>
       </c>
     </row>
@@ -605,21 +605,21 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1096243733</v>
+        <v>1005184329</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>SHAROLL DANIELA</t>
+          <t>WILLIAM ANDRES</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>TORRES CHACON</t>
+          <t>LOPEZ RIOS</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>RETIRO VOLUNTARIO</t>
+          <t>CANCELADO</t>
         </is>
       </c>
     </row>
@@ -630,21 +630,21 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1102348123</v>
+        <v>1005185919</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ELIANA LISETH</t>
+          <t>SEBASTIAN</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>PACHECO BARON</t>
+          <t>PERTUZ SAMPAYO</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>RETIRO VOLUNTARIO</t>
+          <t>CERTIFICADO</t>
         </is>
       </c>
     </row>
@@ -655,21 +655,321 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>57299599</v>
+        <v>1005220651</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LOURDES MARIA</t>
+          <t>BRAYAN EDUARDO</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>OLIVEROS VILLANUEVA</t>
+          <t>BADILLO HERRERA</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1005239745</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>SARAY DUVIANA</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>UNRIZA JAIMES</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1005241421</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>CLARA LUCIA</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>RUIZ MONSALVE</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>RETIRO VOLUNTARIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1043962939</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>DANNA KAROLAY</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>RESTREPO SOSA</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1048457729</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>DAYANA</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>URRUCHURTU NIÑO</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1049019898</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>KAREN YURLEIDY</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>MARIN VARGAS</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>RETIRO VOLUNTARIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1087985197</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>GISELL MARIANA</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>MARIN LARROTA</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1096184002</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>DANIELA</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>ROJAS BOTELLO</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1096186262</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>KEVIN ANDRES</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>PARADA SUAREZ</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>RETIRO VOLUNTARIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1096189477</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>KAMILA</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>QUINTERO CARREÑO</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1097183074</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>MARIA JOSE</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>ORTIZ GUIZA</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1144182405</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>CAROLAIN</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>ABANIS PEREZ</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>63469380</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>VIDA EMPERATRIZ</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>SANTOS YAIN</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se desvinculo instructor de la clase Aprendiz
</commit_message>
<xml_diff>
--- a/novedades.xlsx
+++ b/novedades.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,7 +438,7 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>45359</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="3">
@@ -449,7 +449,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1262805</t>
+          <t>2556845</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CONTABILIDAD Y FINANZAS</t>
+          <t>DISEÑO E INTEGRACION DE MULTIMEDIA</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>42639</v>
+        <v>44760</v>
       </c>
     </row>
     <row r="7">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C7" s="1" t="n">
-        <v>43368</v>
+        <v>45124</v>
       </c>
     </row>
     <row r="8">
@@ -555,16 +555,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1005181647</v>
+        <v>1005178211</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>JOAN MANUEL</t>
+          <t>JUAN CAMILO</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>PALENCIA LOPEZ</t>
+          <t>DELGADO CARRASCAL</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -580,21 +580,21 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1020495471</v>
+        <v>1005181992</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>JOAN MANUEL</t>
+          <t>JOHAN</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>PALENCIA LOPEZ</t>
+          <t>VARGAS CALDERIN</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>CERTIFICADO</t>
+          <t>POR CERTIFICAR</t>
         </is>
       </c>
     </row>
@@ -605,21 +605,21 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1095946925</v>
+        <v>1005184329</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>DANNA GERALDINE</t>
+          <t>WILLIAM ANDRES</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>VEGA SANCHEZ</t>
+          <t>LOPEZ RIOS</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>CERTIFICADO</t>
+          <t>CANCELADO</t>
         </is>
       </c>
     </row>
@@ -630,21 +630,21 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1096189854</v>
+        <v>1005185919</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>LIZETH PAOLA</t>
+          <t>SEBASTIAN</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>LOBO SALCEDO</t>
+          <t>PERTUZ SAMPAYO</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>TRASLADADO</t>
+          <t>CERTIFICADO</t>
         </is>
       </c>
     </row>
@@ -655,16 +655,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1096194400</v>
+        <v>1005220651</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>KATHERINE</t>
+          <t>BRAYAN EDUARDO</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>TERRAZA ALVAREZ</t>
+          <t>BADILLO HERRERA</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -680,16 +680,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1096197940</v>
+        <v>1005239745</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MAYERLY PAOLA</t>
+          <t>SARAY DUVIANA</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>CAÑA PALACIO</t>
+          <t>UNRIZA JAIMES</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -705,21 +705,21 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1096201993</v>
+        <v>1005241421</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>JOHANNA PAOLA</t>
+          <t>CLARA LUCIA</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>BARRERA RODRIGUEZ</t>
+          <t>RUIZ MONSALVE</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>CERTIFICADO</t>
+          <t>RETIRO VOLUNTARIO</t>
         </is>
       </c>
     </row>
@@ -730,16 +730,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1096208435</v>
+        <v>1043962939</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>KAROL VANESSA</t>
+          <t>DANNA KAROLAY</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>ORTEGA TOLOZA</t>
+          <t>RESTREPO SOSA</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -755,16 +755,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1096210258</v>
+        <v>1048457729</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>KAREN MARCELA</t>
+          <t>DAYANA</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>ALVARADO GARCIA</t>
+          <t>URRUCHURTU NIÑO</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -776,25 +776,25 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CC</t>
+          <t>TI</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1096211115</v>
+        <v>1049019898</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>PAOLA ANDREA</t>
+          <t>KAREN YURLEIDY</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>MERCADO MARIN</t>
+          <t>MARIN VARGAS</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>CERTIFICADO</t>
+          <t>RETIRO VOLUNTARIO</t>
         </is>
       </c>
     </row>
@@ -805,16 +805,16 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1096213910</v>
+        <v>1087985197</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>YENIFER PAOLA</t>
+          <t>GISELL MARIANA</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>LEYVA ALVARINO</t>
+          <t>MARIN LARROTA</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -830,21 +830,21 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1096214167</v>
+        <v>1096184002</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>MARYI LISETH</t>
+          <t>DANIELA</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>CHIMA TRIANA</t>
+          <t>ROJAS BOTELLO</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>RETIRO VOLUNTARIO</t>
+          <t>CERTIFICADO</t>
         </is>
       </c>
     </row>
@@ -855,21 +855,21 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1096216042</v>
+        <v>1096186262</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>CHERIL ANDREA</t>
+          <t>KEVIN ANDRES</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>NAVARRO GOMEZ</t>
+          <t>PARADA SUAREZ</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>CERTIFICADO</t>
+          <t>RETIRO VOLUNTARIO</t>
         </is>
       </c>
     </row>
@@ -880,16 +880,16 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1096223641</v>
+        <v>1096189477</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ELSA PAOLA</t>
+          <t>KAMILA</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>VIDES OROZCO</t>
+          <t>QUINTERO CARREÑO</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -905,16 +905,16 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1096223976</v>
+        <v>1097183074</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>KAROL</t>
+          <t>MARIA JOSE</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>BUITRAGO RINCON</t>
+          <t>ORTIZ GUIZA</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -930,16 +930,16 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1096226289</v>
+        <v>1144182405</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>FANNY PAOLA</t>
+          <t>CAROLAIN</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>VALENCIA OSSES</t>
+          <t>ABANIS PEREZ</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -955,519 +955,19 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1096227259</v>
+        <v>63469380</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>JUAN DAVID</t>
+          <t>VIDA EMPERATRIZ</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>JOYA BELLO</t>
+          <t>SANTOS YAIN</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>1096229358</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>LITH JHAJAIRA</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>PUERTA GOMEZ</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>CANCELADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>1096231912</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>LEIDY JOHANNA</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>PEREIRA GARCIA</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>CANCELADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>1096233614</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>KATHERIN</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>DIAZ CASTILLO</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>1096234226</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>ANDRES FELIPE</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>PEREZ SARMIENTO</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>CANCELADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>1096237824</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>JHON MAYRO</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>PATIÑO CASTILLO</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>TRASLADADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>1096238898</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>MANUEL YAIR</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>SILVA DURAN</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>1096240013</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>INGRID VANESSA</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>ARIAS DIAZ</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>CANCELADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>1096242025</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>YURLEY TATIANA</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>CARDONA GARZON</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>1096242447</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>EYLEEN YARITZA</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>GARCIA RUEDA</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>1096248773</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>WINDRY LISNETH</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>ARENAS COLMENARES</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>1096249526</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>JESSICA MELISSA</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>CAMPO MONCADA</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>1096252843</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>ABEL RICARDO</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>MARTINEZ RUEDA</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>1098607019</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>SIRLEY</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>DELGADILLO SIERRA</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>TRASLADADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>1098695412</v>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>RODRIGO ANDRES</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>PEREZ CARRASCAL</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>1098769158</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>BRAYAN SNEIDER</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>GAMARRA ZAPATA</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>28020924</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>YAZMIH LORENA</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>MONTES GALVAN</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>CANCELADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>37577019</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>SANDRA PATRICIA</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>RAMIREZ ECHEVERRY</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>37578408</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>YEIMI</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>AMAYA SUAREZ</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>CANCELADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>37580170</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>VIVIANA</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>RODRIGUEZ MUÑOZ</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>63472623</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>YADIRA</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>HOSTIA SALAS</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
         <is>
           <t>CERTIFICADO</t>
         </is>

</xml_diff>

<commit_message>
Se añadio ajax para documento en seguimientos
</commit_message>
<xml_diff>
--- a/novedades.xlsx
+++ b/novedades.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,7 +438,7 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>45363</v>
+        <v>45364</v>
       </c>
     </row>
     <row r="3">
@@ -449,7 +449,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2711876</t>
+          <t>2556845</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>INTEGRACION DE CONTENIDOS DIGITALES.</t>
+          <t>DISEÑO E INTEGRACION DE MULTIMEDIA</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>45033</v>
+        <v>44760</v>
       </c>
     </row>
     <row r="7">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C7" s="1" t="n">
-        <v>45489</v>
+        <v>45124</v>
       </c>
     </row>
     <row r="8">
@@ -555,21 +555,21 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1096219906</v>
+        <v>1005178211</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CHARLES JAVIER</t>
+          <t>JUAN CAMILO</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>GALO CONTRERAS</t>
+          <t>DELGADO CARRASCAL</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>RETIRO VOLUNTARIO</t>
+          <t>CERTIFICADO</t>
         </is>
       </c>
     </row>
@@ -580,21 +580,21 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1096240059</v>
+        <v>1005181992</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MARIA PAULA</t>
+          <t>JOHAN</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ARTEAGA CARRILLO</t>
+          <t>VARGAS CALDERIN</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>RETIRO VOLUNTARIO</t>
+          <t>POR CERTIFICAR</t>
         </is>
       </c>
     </row>
@@ -605,21 +605,21 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1096243733</v>
+        <v>1005184329</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>SHAROLL DANIELA</t>
+          <t>WILLIAM ANDRES</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>TORRES CHACON</t>
+          <t>LOPEZ RIOS</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>RETIRO VOLUNTARIO</t>
+          <t>CANCELADO</t>
         </is>
       </c>
     </row>
@@ -630,21 +630,21 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1102348123</v>
+        <v>1005185919</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ELIANA LISETH</t>
+          <t>SEBASTIAN</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>PACHECO BARON</t>
+          <t>PERTUZ SAMPAYO</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>RETIRO VOLUNTARIO</t>
+          <t>CERTIFICADO</t>
         </is>
       </c>
     </row>
@@ -655,21 +655,321 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>57299599</v>
+        <v>1005220651</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LOURDES MARIA</t>
+          <t>BRAYAN EDUARDO</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>OLIVEROS VILLANUEVA</t>
+          <t>BADILLO HERRERA</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1005239745</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>SARAY DUVIANA</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>UNRIZA JAIMES</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1005241421</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>CLARA LUCIA</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>RUIZ MONSALVE</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>RETIRO VOLUNTARIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1043962939</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>DANNA KAROLAY</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>RESTREPO SOSA</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1048457729</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>DAYANA</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>URRUCHURTU NIÑO</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1049019898</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>KAREN YURLEIDY</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>MARIN VARGAS</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>RETIRO VOLUNTARIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1087985197</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>GISELL MARIANA</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>MARIN LARROTA</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1096184002</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>DANIELA</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>ROJAS BOTELLO</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1096186262</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>KEVIN ANDRES</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>PARADA SUAREZ</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>RETIRO VOLUNTARIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1096189477</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>KAMILA</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>QUINTERO CARREÑO</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1097183074</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>MARIA JOSE</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>ORTIZ GUIZA</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1144182405</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>CAROLAIN</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>ABANIS PEREZ</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>63469380</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>VIDA EMPERATRIZ</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>SANTOS YAIN</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se unio centro a ficha en vez de seguimientos
</commit_message>
<xml_diff>
--- a/novedades.xlsx
+++ b/novedades.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,7 +438,7 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>45364</v>
+        <v>45365</v>
       </c>
     </row>
     <row r="3">
@@ -449,7 +449,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2556845</t>
+          <t>2711876</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>DISEÑO E INTEGRACION DE MULTIMEDIA</t>
+          <t>INTEGRACION DE CONTENIDOS DIGITALES.</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44760</v>
+        <v>45033</v>
       </c>
     </row>
     <row r="7">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C7" s="1" t="n">
-        <v>45124</v>
+        <v>45489</v>
       </c>
     </row>
     <row r="8">
@@ -555,21 +555,21 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1005178211</v>
+        <v>1096219906</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>JUAN CAMILO</t>
+          <t>CHARLES JAVIER</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>DELGADO CARRASCAL</t>
+          <t>GALO CONTRERAS</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>CERTIFICADO</t>
+          <t>RETIRO VOLUNTARIO</t>
         </is>
       </c>
     </row>
@@ -580,21 +580,21 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1005181992</v>
+        <v>1096240059</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>JOHAN</t>
+          <t>MARIA PAULA</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>VARGAS CALDERIN</t>
+          <t>ARTEAGA CARRILLO</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>POR CERTIFICAR</t>
+          <t>RETIRO VOLUNTARIO</t>
         </is>
       </c>
     </row>
@@ -605,21 +605,21 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1005184329</v>
+        <v>1096243733</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>WILLIAM ANDRES</t>
+          <t>SHAROLL DANIELA</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>LOPEZ RIOS</t>
+          <t>TORRES CHACON</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>CANCELADO</t>
+          <t>RETIRO VOLUNTARIO</t>
         </is>
       </c>
     </row>
@@ -630,21 +630,21 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1005185919</v>
+        <v>1102348123</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>SEBASTIAN</t>
+          <t>ELIANA LISETH</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>PERTUZ SAMPAYO</t>
+          <t>PACHECO BARON</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>CERTIFICADO</t>
+          <t>RETIRO VOLUNTARIO</t>
         </is>
       </c>
     </row>
@@ -655,321 +655,21 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1005220651</v>
+        <v>57299599</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>BRAYAN EDUARDO</t>
+          <t>LOURDES MARIA</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>BADILLO HERRERA</t>
+          <t>OLIVEROS VILLANUEVA</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>1005239745</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>SARAY DUVIANA</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>UNRIZA JAIMES</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>1005241421</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>CLARA LUCIA</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>RUIZ MONSALVE</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
           <t>RETIRO VOLUNTARIO</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>1043962939</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>DANNA KAROLAY</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>RESTREPO SOSA</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>1048457729</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>DAYANA</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>URRUCHURTU NIÑO</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>1049019898</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>KAREN YURLEIDY</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>MARIN VARGAS</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>RETIRO VOLUNTARIO</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>1087985197</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>GISELL MARIANA</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>MARIN LARROTA</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>1096184002</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>DANIELA</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>ROJAS BOTELLO</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>1096186262</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>KEVIN ANDRES</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>PARADA SUAREZ</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>RETIRO VOLUNTARIO</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>1096189477</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>KAMILA</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>QUINTERO CARREÑO</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>1097183074</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>MARIA JOSE</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>ORTIZ GUIZA</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>1144182405</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>CAROLAIN</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>ABANIS PEREZ</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>63469380</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>VIDA EMPERATRIZ</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>SANTOS YAIN</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>CERTIFICADO</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ya trae los demás valores a buscar el aprendiz por cedula.
</commit_message>
<xml_diff>
--- a/novedades.xlsx
+++ b/novedades.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,7 +449,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2711876</t>
+          <t>2556845</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>INTEGRACION DE CONTENIDOS DIGITALES.</t>
+          <t>DISEÑO E INTEGRACION DE MULTIMEDIA</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>45033</v>
+        <v>44760</v>
       </c>
     </row>
     <row r="7">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C7" s="1" t="n">
-        <v>45489</v>
+        <v>45124</v>
       </c>
     </row>
     <row r="8">
@@ -555,21 +555,21 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1096219906</v>
+        <v>1005178211</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CHARLES JAVIER</t>
+          <t>JUAN CAMILO</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>GALO CONTRERAS</t>
+          <t>DELGADO CARRASCAL</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>RETIRO VOLUNTARIO</t>
+          <t>CERTIFICADO</t>
         </is>
       </c>
     </row>
@@ -580,21 +580,21 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1096240059</v>
+        <v>1005181992</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MARIA PAULA</t>
+          <t>JOHAN</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ARTEAGA CARRILLO</t>
+          <t>VARGAS CALDERIN</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>RETIRO VOLUNTARIO</t>
+          <t>POR CERTIFICAR</t>
         </is>
       </c>
     </row>
@@ -605,21 +605,21 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1096243733</v>
+        <v>1005184329</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>SHAROLL DANIELA</t>
+          <t>WILLIAM ANDRES</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>TORRES CHACON</t>
+          <t>LOPEZ RIOS</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>RETIRO VOLUNTARIO</t>
+          <t>CANCELADO</t>
         </is>
       </c>
     </row>
@@ -630,21 +630,21 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1102348123</v>
+        <v>1005185919</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ELIANA LISETH</t>
+          <t>SEBASTIAN</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>PACHECO BARON</t>
+          <t>PERTUZ SAMPAYO</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>RETIRO VOLUNTARIO</t>
+          <t>CERTIFICADO</t>
         </is>
       </c>
     </row>
@@ -655,21 +655,321 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>57299599</v>
+        <v>1005220651</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LOURDES MARIA</t>
+          <t>BRAYAN EDUARDO</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>OLIVEROS VILLANUEVA</t>
+          <t>BADILLO HERRERA</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1005239745</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>SARAY DUVIANA</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>UNRIZA JAIMES</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1005241421</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>CLARA LUCIA</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>RUIZ MONSALVE</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>RETIRO VOLUNTARIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1043962939</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>DANNA KAROLAY</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>RESTREPO SOSA</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1048457729</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>DAYANA</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>URRUCHURTU NIÑO</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1049019898</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>KAREN YURLEIDY</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>MARIN VARGAS</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>RETIRO VOLUNTARIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1087985197</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>GISELL MARIANA</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>MARIN LARROTA</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1096184002</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>DANIELA</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>ROJAS BOTELLO</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1096186262</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>KEVIN ANDRES</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>PARADA SUAREZ</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>RETIRO VOLUNTARIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1096189477</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>KAMILA</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>QUINTERO CARREÑO</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1097183074</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>MARIA JOSE</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>ORTIZ GUIZA</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1144182405</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>CAROLAIN</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>ABANIS PEREZ</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>63469380</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>VIDA EMPERATRIZ</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>SANTOS YAIN</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>CERTIFICADO</t>
         </is>
       </c>
     </row>

</xml_diff>